<commit_message>
Changed output names in xlsx files for Ligules
</commit_message>
<xml_diff>
--- a/Tests/Validation/Barley/Observations/MCPD11_12Leaves.xlsx
+++ b/Tests/Validation/Barley/Observations/MCPD11_12Leaves.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\ApsimX\Prototypes\Barley\Observations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ApsimX\Tests\Validation\Barley\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBAC1DE-ED94-4979-86D6-C59DFA260137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +34,6 @@
   </si>
   <si>
     <t>Barley.Structure.LeafTipsAppeared</t>
-  </si>
-  <si>
-    <t>Barley.Leaf.ExpandedCohortNo</t>
   </si>
   <si>
     <t>Tillers_perPlant</t>
@@ -70,11 +68,14 @@
   <si>
     <t>MCPD11_12CultOmakaSD3</t>
   </si>
+  <si>
+    <t>Barley.Leaf.Ligules</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -390,19 +391,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E67"/>
+      <selection activeCell="D1" sqref="A1:E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,15 +414,15 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>40780</v>
@@ -436,9 +437,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>40787</v>
@@ -450,12 +451,12 @@
         <v>1.5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>40795</v>
@@ -470,9 +471,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>40802</v>
@@ -487,9 +488,9 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>40810</v>
@@ -504,9 +505,9 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>40816</v>
@@ -521,9 +522,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>40827</v>
@@ -535,12 +536,12 @@
         <v>5.6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
         <v>40833</v>
@@ -552,12 +553,12 @@
         <v>6.45</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
         <v>40844</v>
@@ -569,12 +570,12 @@
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1">
         <v>40855</v>
@@ -586,12 +587,12 @@
         <v>10.55</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
       </c>
       <c r="B12" s="1">
         <v>40780</v>
@@ -606,9 +607,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
         <v>40787</v>
@@ -620,12 +621,12 @@
         <v>1.4</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
       </c>
       <c r="B14" s="1">
         <v>40795</v>
@@ -640,9 +641,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1">
         <v>40802</v>
@@ -657,9 +658,9 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1">
         <v>40810</v>
@@ -674,9 +675,9 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1">
         <v>40816</v>
@@ -691,9 +692,9 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1">
         <v>40827</v>
@@ -705,12 +706,12 @@
         <v>5.6</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
       </c>
       <c r="B19" s="1">
         <v>40833</v>
@@ -722,12 +723,12 @@
         <v>6.1578947368421053</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>7</v>
       </c>
       <c r="B20" s="1">
         <v>40844</v>
@@ -739,12 +740,12 @@
         <v>7.75</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>7</v>
       </c>
       <c r="B21" s="1">
         <v>40855</v>
@@ -756,12 +757,12 @@
         <v>10.15</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1">
         <v>40780</v>
@@ -776,9 +777,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1">
         <v>40787</v>
@@ -790,12 +791,12 @@
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="1">
         <v>40795</v>
@@ -810,9 +811,9 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="1">
         <v>40802</v>
@@ -827,9 +828,9 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" s="1">
         <v>40810</v>
@@ -844,9 +845,9 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" s="1">
         <v>40816</v>
@@ -861,9 +862,9 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1">
         <v>40827</v>
@@ -875,12 +876,12 @@
         <v>5.7</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" s="1">
         <v>40833</v>
@@ -892,12 +893,12 @@
         <v>6.45</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" s="1">
         <v>40844</v>
@@ -909,12 +910,12 @@
         <v>7.85</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31" s="1">
         <v>40855</v>
@@ -926,12 +927,12 @@
         <v>10.3</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" s="1">
         <v>40816</v>
@@ -943,12 +944,12 @@
         <v>0</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" s="1">
         <v>40827</v>
@@ -960,12 +961,12 @@
         <v>1.9</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" s="1">
         <v>40833</v>
@@ -980,9 +981,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" s="1">
         <v>40844</v>
@@ -994,12 +995,12 @@
         <v>4.05</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="1">
         <v>40855</v>
@@ -1011,12 +1012,12 @@
         <v>6</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" s="1">
         <v>40863</v>
@@ -1028,12 +1029,12 @@
         <v>7.8</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" s="1">
         <v>40878</v>
@@ -1045,12 +1046,12 @@
         <v>10.4</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" s="1">
         <v>40816</v>
@@ -1062,12 +1063,12 @@
         <v>0</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" s="1">
         <v>40827</v>
@@ -1079,12 +1080,12 @@
         <v>2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41" s="1">
         <v>40833</v>
@@ -1099,9 +1100,9 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" s="1">
         <v>40844</v>
@@ -1113,12 +1114,12 @@
         <v>4</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43" s="1">
         <v>40855</v>
@@ -1130,12 +1131,12 @@
         <v>5.85</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" s="1">
         <v>40863</v>
@@ -1147,12 +1148,12 @@
         <v>7.4</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B45" s="1">
         <v>40878</v>
@@ -1164,12 +1165,12 @@
         <v>10.1</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46" s="1">
         <v>40816</v>
@@ -1181,12 +1182,12 @@
         <v>0</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" s="1">
         <v>40827</v>
@@ -1198,12 +1199,12 @@
         <v>2</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" s="1">
         <v>40833</v>
@@ -1218,9 +1219,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" s="1">
         <v>40844</v>
@@ -1232,12 +1233,12 @@
         <v>4</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="1">
         <v>40855</v>
@@ -1249,12 +1250,12 @@
         <v>5.45</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" s="1">
         <v>40863</v>
@@ -1266,12 +1267,12 @@
         <v>6.8</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52" s="1">
         <v>40878</v>
@@ -1283,12 +1284,12 @@
         <v>9.8333333333333339</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B53" s="1">
         <v>40882</v>
@@ -1300,12 +1301,12 @@
         <v>2.7</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" s="1">
         <v>40889</v>
@@ -1317,12 +1318,12 @@
         <v>4</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55" s="1">
         <v>40897</v>
@@ -1334,12 +1335,12 @@
         <v>5.2</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B56" s="1">
         <v>40907</v>
@@ -1351,12 +1352,12 @@
         <v>7.8947368421052628</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B57" s="1">
         <v>40919</v>
@@ -1368,12 +1369,12 @@
         <v>9.3157894736842106</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B58" s="1">
         <v>40882</v>
@@ -1385,12 +1386,12 @@
         <v>2.85</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B59" s="1">
         <v>40889</v>
@@ -1402,12 +1403,12 @@
         <v>4</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B60" s="1">
         <v>40897</v>
@@ -1419,12 +1420,12 @@
         <v>5</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B61" s="1">
         <v>40907</v>
@@ -1436,12 +1437,12 @@
         <v>7.6</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B62" s="1">
         <v>40919</v>
@@ -1453,12 +1454,12 @@
         <v>9.4666666666666668</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B63" s="1">
         <v>40882</v>
@@ -1470,12 +1471,12 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B64" s="1">
         <v>40889</v>
@@ -1487,12 +1488,12 @@
         <v>4</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B65" s="1">
         <v>40897</v>
@@ -1504,12 +1505,12 @@
         <v>4.9411764705882355</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B66" s="1">
         <v>40907</v>
@@ -1521,12 +1522,12 @@
         <v>7.0714285714285712</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B67" s="1">
         <v>40919</v>
@@ -1538,7 +1539,7 @@
         <v>8.7777777777777786</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>